<commit_message>
added 2 spreadsheets in Grade 9 and a .docx in Grade8
</commit_message>
<xml_diff>
--- a/Grade9/ExcelPracticeGade9.xlsx
+++ b/Grade9/ExcelPracticeGade9.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="ProductSales" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -192,12 +194,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -211,6 +217,92 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>290880</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>43560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2729160" cy="3782520"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>430200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>102240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 2"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="2868480" cy="2865600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,252 +485,300 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="14.25" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="1" t="n">
+      <c r="C12" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="1" t="n">
+      <c r="C13" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="n">
+      <c r="C14" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>